<commit_message>
Refaktoring przed zdaniem ukończonego projektu
</commit_message>
<xml_diff>
--- a/ExcelPln2/Input/Test17102016/BAT__test.xlsx
+++ b/ExcelPln2/Input/Test17102016/BAT__test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="245" yWindow="258" windowWidth="20119" windowHeight="7811" activeTab="1"/>
+    <workbookView xWindow="245" yWindow="258" windowWidth="20119" windowHeight="7811"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="7" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>PLANOGRAM</t>
   </si>
@@ -219,18 +219,6 @@
     <t>Prince Rich Taste
  3594</t>
   </si>
-  <si>
-    <t>JIII Sobieski Czerwony 
-792</t>
-  </si>
-  <si>
-    <t>JIII Sobieski Niebieski
-793</t>
-  </si>
-  <si>
-    <t>JIII Sobieski Błękitny
-794</t>
-  </si>
 </sst>
 </file>
 
@@ -363,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -438,17 +426,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -467,7 +444,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -590,9 +567,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="=D:\WINNT\SYSTEM32\COMMAND.COM" xfId="4"/>
@@ -694,210 +668,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1209675</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 71"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="486134" y="8015917"/>
-          <a:ext cx="542925" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1200150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 72"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1294681" y="8015917"/>
-          <a:ext cx="551372" cy="904875"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>267599</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>573117</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>62900</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1468467</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 73"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4552052" y="8279380"/>
-          <a:ext cx="542925" cy="895350"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -917,7 +687,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -985,7 +755,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1121,7 +891,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1189,7 +959,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1257,7 +1027,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1325,7 +1095,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1393,7 +1163,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1461,7 +1231,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1529,7 +1299,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1597,7 +1367,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1665,7 +1435,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1733,7 +1503,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1801,7 +1571,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1869,7 +1639,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1937,7 +1707,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2000,7 +1770,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2063,7 +1833,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2126,7 +1896,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2189,7 +1959,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2252,7 +2022,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2315,7 +2085,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2378,7 +2148,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2441,7 +2211,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2509,7 +2279,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2577,7 +2347,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2645,7 +2415,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2713,7 +2483,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2776,7 +2546,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2839,7 +2609,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2907,7 +2677,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2975,7 +2745,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3043,7 +2813,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3111,7 +2881,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3179,7 +2949,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3247,7 +3017,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3315,7 +3085,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3383,7 +3153,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3451,7 +3221,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3519,7 +3289,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3587,7 +3357,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3655,7 +3425,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3723,7 +3493,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3791,7 +3561,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3859,7 +3629,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3927,7 +3697,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3995,7 +3765,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4063,7 +3833,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4131,7 +3901,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4199,7 +3969,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4267,7 +4037,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4335,7 +4105,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4403,7 +4173,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4471,7 +4241,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4539,7 +4309,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4607,7 +4377,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4675,7 +4445,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4743,7 +4513,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4811,7 +4581,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4879,7 +4649,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4947,7 +4717,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5015,7 +4785,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5083,7 +4853,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5151,7 +4921,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5219,7 +4989,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5287,7 +5057,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5355,7 +5125,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5423,7 +5193,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5491,7 +5261,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5559,7 +5329,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5627,7 +5397,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5695,7 +5465,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5763,7 +5533,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5831,7 +5601,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5899,7 +5669,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5967,7 +5737,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6035,7 +5805,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6103,7 +5873,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6171,7 +5941,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6239,7 +6009,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6307,7 +6077,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6375,7 +6145,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6443,7 +6213,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6511,7 +6281,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6579,7 +6349,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6647,7 +6417,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6715,7 +6485,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6783,7 +6553,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -7136,11 +6906,14 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7178,8 +6951,8 @@
   </sheetPr>
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -7569,21 +7342,15 @@
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="39"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
@@ -7793,7 +7560,7 @@
       <c r="AA14" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
@@ -7802,7 +7569,6 @@
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="D8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>